<commit_message>
xlsx and pdf revised
</commit_message>
<xml_diff>
--- a/prepa_certif.xlsx
+++ b/prepa_certif.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\principal\Desktop\prepa_certif\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01DEF4EB-D304-4496-B79F-CD1C837312FF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{474FDF90-7EBA-48DF-B5DC-BB7D5695F9BD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="21320" yWindow="1340" windowWidth="16030" windowHeight="17740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Burndown chart</t>
   </si>
@@ -80,9 +80,6 @@
   </si>
   <si>
     <t>scrum team</t>
-  </si>
-  <si>
-    <t>différentes équipes scrum d'un même produit peuvent NE PAS avoir des sprints de longueur différente. (does not require)</t>
   </si>
   <si>
     <t>Scrum artifacts</t>
@@ -148,6 +145,16 @@
   </si>
   <si>
     <t>sprint backlog, product backlog, increment.      PILARS : Transparency, adaptation, inspection</t>
+  </si>
+  <si>
+    <t>différentes équipes scrum d'un même produit peuvent NE PAS avoir des sprints de longueur différente. (does not require)
+Elle fait le SPRINT PLANNING.</t>
+  </si>
+  <si>
+    <t>Sprint planning</t>
+  </si>
+  <si>
+    <t>La scrum team peut y assister.</t>
   </si>
 </sst>
 </file>
@@ -574,10 +581,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.5" x14ac:dyDescent="0.35"/>
@@ -590,7 +597,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="40" customHeight="1" x14ac:dyDescent="0.35">
@@ -650,58 +657,69 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" s="3"/>
+    </row>
+    <row r="14" spans="1:2" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="3"/>
+    </row>
+    <row r="16" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B18" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="58" x14ac:dyDescent="0.35">
-      <c r="A16" s="3" t="s">
+    <row r="20" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+      <c r="A20" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="3"/>
-    </row>
-    <row r="18" spans="1:2" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18" s="2" t="s">
+      <c r="B20" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="14" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A20" s="3" t="s">
+    <row r="21" spans="1:2" ht="14" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B22" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="14" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="22" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A22" s="3" t="s">
+    <row r="23" spans="1:2" ht="14" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="24" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A24" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A24" s="3" t="s">
-        <v>19</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
revision end of 1st psm1
</commit_message>
<xml_diff>
--- a/prepa_certif.xlsx
+++ b/prepa_certif.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\principal\Desktop\prepa_certif\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F8A6440-322C-4E5A-871D-0BB8575E9A35}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{141B82F7-178D-4D5E-8188-DB59C6F12B34}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="21140" yWindow="240" windowWidth="16030" windowHeight="20600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Burndown chart</t>
   </si>
@@ -101,125 +101,7 @@
 déviation</t>
   </si>
   <si>
-    <t>Un burndown chart ou BDC : représentation graphique de l'évolution de quantité de travail restante par rapport au temps sur une période de temps donnée. Responsable : dev team.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">De l'incertitude vers de la meilleure connaissance sur le projet. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>SI déviation</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> &gt;&gt;&gt; correction au + vite.</t>
-    </r>
-  </si>
-  <si>
     <t>le PO, dev team. "consume not more than 10%"</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>cancellation</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> : PO only,  la qualité ne doit pas baisser, l'objectif ne doit pas être mis en danger.</t>
-    </r>
-  </si>
-  <si>
-    <t>But : présenter le produit (travail réalisé) durant le sprint en cours OU après un product backlog révisé. 
-C'est pour les key stakeholders, scrum master, dev team, PO.</t>
-  </si>
-  <si>
-    <t>Cérémonie scrum en fermeture du sprint qui se réalise juste après la sprint Review. C'est pour la dev team. 
-Sert à l'amélioration pour les prochains sprints, analyse ce qui s'est passé &gt;&gt; people, relationships, process, and tool.</t>
-  </si>
-  <si>
-    <t>Dev team, 15 minutes peu importe la taille de l'équipe, le scrum master ne la "conduit" pas, 
-3 questions du scrum master : je vois les obstacles qui empêchent d'aller au but, j'ai vu hier ce qui peut aider la dev team, je peux les aider aujourd'hui à atteindre ce but. --NO CANCELLATION ALLOWED--.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Dev team (responsable du suivi du travail restant), la définition de "done" peut possiblement s'adapter à chaque RETRO par la scrum team, n'aide pas à calculer la vélocité.
-DONE est l'objectif, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>pas la réduction de la dette technique par un sprint spécial</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">The Product Backlog items selected for this sprint plus the plan for delivering them. 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>changes during sprint:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> dev team ONLY (belongs solely).</t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">Scrum master, product owner, dev team.  
@@ -304,6 +186,137 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">The Product Backlog items selected for this sprint plus the plan for delivering them. 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>changes during sprint:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> dev team ONLY (belongs solely).
+Utiliser la fin du dernier sprint pour plannifier </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>les premiers jours</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> du nouveau sprint.</t>
+    </r>
+  </si>
+  <si>
+    <t>Le PO</t>
+  </si>
+  <si>
+    <t>Interêts : le produit, la valeur, les key stakholder.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>cancellation</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : PO only (&amp; if sprint goal obsolete),  la qualité ne doit pas baisser, l'objectif ne doit pas être mis en danger.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Dev team (responsable du suivi du travail restant), la définition de "done" peut possiblement </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>s'adapter</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> à chaque RETRO par la scrum team, n'aide pas à calculer la vélocité.
+DONE est l'objectif, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>pas la réduction de la dette technique par un sprint spécial (hardening)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.
+Doit respecter : conventions &amp; standards, same definition for other teams working on the same product.</t>
+    </r>
+  </si>
+  <si>
+    <t>Un burndown chart ou BDC : représentation graphique, shows the evolution of remaining effort against time.
+Responsable : dev team.</t>
+  </si>
+  <si>
+    <r>
       <rPr>
         <b/>
         <sz val="12"/>
@@ -322,7 +335,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> : n'est pas adaptable aux projets car chaque composent sert un objectif spécifique.
+      <t xml:space="preserve"> : n'est pas adaptable aux projets car chaque composant sert un objectif spécifique.
 </t>
     </r>
     <r>
@@ -366,12 +379,39 @@
         <scheme val="minor"/>
       </rPr>
       <t>: product backlog re-estimated under PO supervision.
-No titles for dev team members &amp; no sub-teams, accountability belongs to the dev team.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">La scrum team en est responsable, ce n'est pas la place des key stakeholders mais ils peuvent y assister.
+No titles for dev team members &amp; no sub-teams, accountability belongs to the dev team.
+Courage, openness, focus, commitment, respect. Most important : a small team flexible and adaptative.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">How much is known about the Product over time . </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SI déviation</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> &gt;&gt;&gt; correction au + vite.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">8 heures max, la scrum team en est responsable, ce n'est pas la place des key stakeholders mais ils peuvent y assister.
 Participants : la scrum team (scrum master, product owner, dev team).
 Quel est le livrable du prochain increment et comment réaliser le travail pour y parvenir.
 </t>
@@ -396,6 +436,42 @@
         <scheme val="minor"/>
       </rPr>
       <t>: last sprint, product backlog, past performance, last increment.</t>
+    </r>
+  </si>
+  <si>
+    <t>4 heures max, but : présenter le produit (travail réalisé) durant le sprint en cours OU après un product backlog révisé. 
+C'est pour les key stakeholders, scrum master, dev team, PO.</t>
+  </si>
+  <si>
+    <t>3 heures max, cérémonie scrum en fermeture du sprint qui se réalise juste après la sprint Review. C'est pour la dev team. 
+Sert à l'amélioration pour les prochains sprints, analyse ce qui s'est passé &gt;&gt; people, relationships, process, and tool.</t>
+  </si>
+  <si>
+    <r>
+      <t>Dev team, 15 minutes peu importe la taille de l'équipe, le scrum master ne la "conduit" pas.
+PAS DE FORMAT DEFINI</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : questions ou discussion, tout est possible.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+3 questions du scrum master : je vois les obstacles qui empêchent d'aller au but, j'ai vu hier ce qui peut aider la dev team, je peux les aider aujourd'hui à atteindre ce but. --NO CANCELLATION ALLOWED--.</t>
     </r>
   </si>
 </sst>
@@ -833,10 +909,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B29"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.5" x14ac:dyDescent="0.35"/>
@@ -857,7 +933,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="12.5" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -866,7 +942,7 @@
         <v>15</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="12.5" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -875,7 +951,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="12.5" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -884,7 +960,7 @@
         <v>12</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="12.5" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -893,7 +969,7 @@
         <v>1</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="12.5" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -902,16 +978,16 @@
         <v>2</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="12.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="1:2" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="12.5" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -920,16 +996,16 @@
         <v>11</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="12.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="18" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="12.5" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -938,11 +1014,11 @@
         <v>4</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="12.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="22" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
         <v>5</v>
       </c>
@@ -956,7 +1032,7 @@
         <v>7</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="12.5" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -969,15 +1045,23 @@
       </c>
     </row>
     <row r="27" spans="1:2" ht="12.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="28" spans="1:2" ht="45.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" ht="60" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="12.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
revision end of 2nd psm1
</commit_message>
<xml_diff>
--- a/prepa_certif.xlsx
+++ b/prepa_certif.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\principal\Desktop\prepa_certif\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.0.13\Desktop\prepa_certif\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{141B82F7-178D-4D5E-8188-DB59C6F12B34}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{734F7C98-3A61-4E7B-84B0-002458446625}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21140" yWindow="240" windowWidth="16030" windowHeight="20600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Burndown chart</t>
   </si>
@@ -69,8 +69,170 @@
     <t xml:space="preserve">Scrum </t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">sprint backlog, product backlog, increment.      
+    <t>Le PO</t>
+  </si>
+  <si>
+    <t>Interêts : le produit, la valeur, les key stakholder.</t>
+  </si>
+  <si>
+    <t>the Key Stakeholders</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">How much is known about the Product over time . </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SI déviation</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> &gt;&gt;&gt; correction "as soon as possible".</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Scrum master, product owner, dev team.  
+Différentes équipes scrum d'un même produit peuvent NE PAS avoir des sprints de longueur différente. (does not require)
+Elle fait le SPRINT PLANNING, responsible for </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>crafting the sprint goal</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> during it. Elle doit être autosuffisante.
+Qualités importantes : flexibility, creativity, productivity.
+Should have all competencies, should choose how best to accomplish their work.
+</t>
+    </r>
+  </si>
+  <si>
+    <t>allowed : The Sprint Review.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Dev team (responsable du suivi du travail restant), la définition de "done" </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>créée par la dev team</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> peut possiblement </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>s'adapter</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> à chaque RETRO </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>par la scrum team</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, n'aide pas à calculer la vélocité.
+DONE est l'objectif, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>pas la réduction de la dette technique par un sprint spécial (hardening)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.
+Doit respecter : conventions &amp; standards, same definition for other teams working on the same product.
+ensures artifact transparency, is used to acces, guides the dev team.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">sprint backlog, product backlog, increment.   
+Inspect frequently, but it should not get in the way of the work.   
 PILARS : Transparency (responsable scrum master), adaptation, inspection. Le PO monitore.
 </t>
     </r>
@@ -93,27 +255,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> : somme de tous les product backlog items, fait par la dev team.</t>
-    </r>
-  </si>
-  <si>
-    <t>cône d'incertitude
-déviation</t>
-  </si>
-  <si>
-    <t>le PO, dev team. "consume not more than 10%"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Scrum master, product owner, dev team.  
-Différentes équipes scrum d'un même produit peuvent NE PAS avoir des sprints de longueur différente. (does not require)
-Elle fait le SPRINT PLANNING. Elle doit être autosuffisante.
-Qualités importantes : flexibility, creativity, productivity.
-</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Responsable: PO uniquement  
-La dev team peut faire des changements </t>
+      <t xml:space="preserve"> : somme de tous les product backlog items and the value, </t>
     </r>
     <r>
       <rPr>
@@ -124,196 +266,18 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>avec l'accord du PO (attention au sens de la question)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-La dev team est responsable des estimations
-dev teams </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>should</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> use the same product backlog
-&gt; dynamic, never complete, existe tant que le produit existe.
-C'est la seule source pour tout changement du produit.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Management</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> : Ordering items, optimizing value, keep visible &amp; transparent the work on next.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">The Product Backlog items selected for this sprint plus the plan for delivering them. 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>changes during sprint:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> dev team ONLY (belongs solely).
-Utiliser la fin du dernier sprint pour plannifier </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>les premiers jours</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> du nouveau sprint.</t>
-    </r>
-  </si>
-  <si>
-    <t>Le PO</t>
-  </si>
-  <si>
-    <t>Interêts : le produit, la valeur, les key stakholder.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>cancellation</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> : PO only (&amp; if sprint goal obsolete),  la qualité ne doit pas baisser, l'objectif ne doit pas être mis en danger.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Dev team (responsable du suivi du travail restant), la définition de "done" peut possiblement </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>s'adapter</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> à chaque RETRO par la scrum team, n'aide pas à calculer la vélocité.
-DONE est l'objectif, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>pas la réduction de la dette technique par un sprint spécial (hardening)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.
-Doit respecter : conventions &amp; standards, same definition for other teams working on the same product.</t>
-    </r>
-  </si>
-  <si>
-    <t>Un burndown chart ou BDC : représentation graphique, shows the evolution of remaining effort against time.
-Responsable : dev team.</t>
+      <t>fait par la dev team,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> sprint goal provides guidance.</t>
+    </r>
   </si>
   <si>
     <r>
@@ -380,40 +344,290 @@
       </rPr>
       <t>: product backlog re-estimated under PO supervision.
 No titles for dev team members &amp; no sub-teams, accountability belongs to the dev team.
-Courage, openness, focus, commitment, respect. Most important : a small team flexible and adaptative.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">How much is known about the Product over time . </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>SI déviation</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> &gt;&gt;&gt; correction au + vite.</t>
+Courage, openness, focus, commitment, respect.        ESSENCE : a small team flexible and adaptative.
+Scrum can be used EVERYWHERE. Scrum Master usually does care about those outside the Scrum Team.
+les 4 : role, events, artifacts, rules.</t>
+    </r>
+  </si>
+  <si>
+    <t>Le Scrum Master</t>
+  </si>
+  <si>
+    <t>Un burndown chart : How much work remains till the end of the sprint, shows the evolution of remaining effort against time.
+Responsable : dev team.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Helping dev team to create value, removing impediments, coaching the dev team.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Is responsible for conducting the Daily Scrum.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Leading &amp; coaching org, working with other scrum masters, planning scrum implementations.</t>
+    </r>
+  </si>
+  <si>
+    <t>Cône d'incertitude,
+déviation</t>
+  </si>
+  <si>
+    <t>Le PO, dev team. "consume not more than 10%"</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Cancellation</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : PO only (OR </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>if sprint goal obsolete</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">).
+La qualité ne doit pas baisser, l'objectif ne doit pas être mis en danger, scope may be clarified and re-negociated.
+Le sprint est le SEUL moment dans lequel </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>on n'inspecte pas et on n'adapte pas</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>4 heures max, but : présenter le produit (travail réalisé) durant le sprint en cours OU "a revisited product backlog". 
+C'est pour les key stakeholders, scrum master, dev team, PO.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">3 heures max, cérémonie scrum en fermeture du sprint qui se réalise juste après la sprint Review. C'est pour la dev team. 
+Sert à </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>améliorer</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> pour les prochains sprints, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>identifier</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ce qui a été bien et qui a du potentiel d'amélioration, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>analyser</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ce qui s'est passé &gt;&gt; people, relationships, process, and tool.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The Product Backlog items selected for this sprint + the plan for delivering them. 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>changes during sprint:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> dev team ONLY (belongs solely, </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>possible to add new work</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">).
+Utiliser la fin du dernier sprint pour plannifier </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>les premiers jours</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> du nouveau sprint.</t>
     </r>
   </si>
   <si>
     <r>
       <t xml:space="preserve">8 heures max, la scrum team en est responsable, ce n'est pas la place des key stakeholders mais ils peuvent y assister.
-Participants : la scrum team (scrum master, product owner, dev team).
-Quel est le livrable du prochain increment et comment réaliser le travail pour y parvenir.
+Participants : la scrum team (scrum master, product owner, dev team). Others possible to provide </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>technical advice</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">.
+Comment le travail sera fait pour le prochain increment ? (work needed to deliver)
+Qu'est-ce qui sera livré? (delivered in the Increment resulting).
 </t>
     </r>
     <r>
@@ -425,31 +639,45 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">its input </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: last sprint, product backlog, past performance, last increment.</t>
-    </r>
-  </si>
-  <si>
-    <t>4 heures max, but : présenter le produit (travail réalisé) durant le sprint en cours OU après un product backlog révisé. 
-C'est pour les key stakeholders, scrum master, dev team, PO.</t>
-  </si>
-  <si>
-    <t>3 heures max, cérémonie scrum en fermeture du sprint qui se réalise juste après la sprint Review. C'est pour la dev team. 
-Sert à l'amélioration pour les prochains sprints, analyse ce qui s'est passé &gt;&gt; people, relationships, process, and tool.</t>
-  </si>
-  <si>
-    <r>
-      <t>Dev team, 15 minutes peu importe la taille de l'équipe, le scrum master ne la "conduit" pas.
-PAS DE FORMAT DEFINI</t>
+      <t xml:space="preserve">input </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: last sprint, product backlog, past performance, last increment.
+L'important est la plannification </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>des premiers jours</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Dev team, 15 minutes peu importe la taille de l'équipe, le scrum master ne la "conduit" pas.
+PAS DE FORMAT DEFINI : </t>
     </r>
     <r>
       <rPr>
@@ -460,7 +688,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> : questions ou discussion, tout est possible.</t>
+      <t>questions ou discussion, tout est possible.</t>
     </r>
     <r>
       <rPr>
@@ -472,6 +700,122 @@
       </rPr>
       <t xml:space="preserve">
 3 questions du scrum master : je vois les obstacles qui empêchent d'aller au but, j'ai vu hier ce qui peut aider la dev team, je peux les aider aujourd'hui à atteindre ce but. --NO CANCELLATION ALLOWED--.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Responsable: PO uniquement.
+La dev team peut faire des changements </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>avec l'accord du PO (attention au sens de la question)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+La dev team est responsable des </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>estimations.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+dev teams </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>should</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> use the same product backlog.
+&gt; dynamic, never complete, existe tant que le produit existe.
+C'est </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>la seule source</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> pour tout changement du produit.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Management</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : Ordering items, optimizing value, keep visible &amp; transparent the work on next.</t>
     </r>
   </si>
 </sst>
@@ -479,7 +823,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -523,6 +867,14 @@
       <b/>
       <i/>
       <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -909,26 +1261,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:B35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="18" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.08984375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="103.90625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="15.1796875" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="23.109375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="103.88671875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="15.21875" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B1" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -936,132 +1288,151 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="12.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="1:2" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" ht="12.45" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:2" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="12.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="6" spans="1:2" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="12.45" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:2" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="12.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="8" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="12.45" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:2" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="12.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="10" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="12.45" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="12.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="12" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="12.45" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:2" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="12.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="12.45" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="12.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="16" spans="1:2" ht="60.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="12.45" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:2" ht="88.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="12.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="18" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="12.45" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="18" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="12.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="20" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="12.45" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="12.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="22" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="12.45" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="12.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="24" spans="1:2" ht="73" customHeight="1" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="12.45" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="1:2" ht="84" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="12.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="26" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="12.45" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="12.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="28" spans="1:2" ht="60" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="12.45" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="1:2" ht="88.8" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B28" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="12.45" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="12.6" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="12.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A30" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
+    <row r="33" spans="1:2" ht="12.6" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="34" spans="1:2" ht="36" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>